<commit_message>
validate dates and phone numbers and refactor
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FC9456-CD3B-8C40-9EDD-07E10832DEB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FAEA84-37F7-794C-9C1F-2E618D357D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="343">
   <si>
     <t>First Name</t>
   </si>
@@ -634,9 +634,6 @@
     <t>Rohanshire</t>
   </si>
   <si>
-    <t>Lake Lucas</t>
-  </si>
-  <si>
     <t>Grimesmouth</t>
   </si>
   <si>
@@ -700,9 +697,6 @@
     <t>Garfieldstad</t>
   </si>
   <si>
-    <t>Fadelfurt</t>
-  </si>
-  <si>
     <t>Port Lionel</t>
   </si>
   <si>
@@ -1052,6 +1046,9 @@
   </si>
   <si>
     <t>positive</t>
+  </si>
+  <si>
+    <t>Texas</t>
   </si>
 </sst>
 </file>
@@ -1404,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CQ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CD1" workbookViewId="0">
-      <selection activeCell="CJ9" sqref="CJ9"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="BK1" workbookViewId="0">
+      <selection activeCell="BO12" sqref="BO12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1764,34 +1761,34 @@
         <v>84</v>
       </c>
       <c r="CH1" t="s">
+        <v>316</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>317</v>
+      </c>
+      <c r="CJ1" t="s">
         <v>318</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CK1" t="s">
         <v>319</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CL1" t="s">
         <v>320</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CM1" t="s">
         <v>321</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CN1" t="s">
         <v>322</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CO1" t="s">
         <v>323</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CP1" t="s">
         <v>324</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CQ1" t="s">
         <v>325</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>326</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:95" x14ac:dyDescent="0.15">
@@ -1844,7 +1841,7 @@
         <v>95</v>
       </c>
       <c r="Q2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="R2" t="s">
         <v>94</v>
@@ -2329,22 +2326,22 @@
         <v>118</v>
       </c>
       <c r="CH3" t="s">
+        <v>328</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>327</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>329</v>
+      </c>
+      <c r="CK3" t="s">
         <v>330</v>
       </c>
-      <c r="CI3" t="s">
-        <v>329</v>
-      </c>
-      <c r="CJ3" t="s">
+      <c r="CL3" t="s">
         <v>331</v>
       </c>
-      <c r="CK3" t="s">
+      <c r="CM3" t="s">
         <v>332</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>333</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>334</v>
       </c>
       <c r="CN3" t="s">
         <v>94</v>
@@ -2610,34 +2607,34 @@
         <v>118</v>
       </c>
       <c r="CH4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="CI4" t="s">
+        <v>327</v>
+      </c>
+      <c r="CJ4" t="s">
         <v>329</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CK4" t="s">
+        <v>333</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>334</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>332</v>
+      </c>
+      <c r="CN4" t="s">
+        <v>329</v>
+      </c>
+      <c r="CO4" t="s">
+        <v>226</v>
+      </c>
+      <c r="CP4" t="s">
         <v>331</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CQ4" t="s">
         <v>335</v>
-      </c>
-      <c r="CL4" t="s">
-        <v>336</v>
-      </c>
-      <c r="CM4" t="s">
-        <v>334</v>
-      </c>
-      <c r="CN4" t="s">
-        <v>331</v>
-      </c>
-      <c r="CO4" t="s">
-        <v>228</v>
-      </c>
-      <c r="CP4" t="s">
-        <v>333</v>
-      </c>
-      <c r="CQ4" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:95" x14ac:dyDescent="0.15">
@@ -2690,7 +2687,7 @@
         <v>171</v>
       </c>
       <c r="Q5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="R5" t="s">
         <v>94</v>
@@ -2891,10 +2888,10 @@
         <v>94</v>
       </c>
       <c r="CH5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="CI5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:95" x14ac:dyDescent="0.15">
@@ -3079,13 +3076,13 @@
         <v>203</v>
       </c>
       <c r="BI6" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>94</v>
+      </c>
+      <c r="BK6" t="s">
         <v>204</v>
-      </c>
-      <c r="BJ6" t="s">
-        <v>94</v>
-      </c>
-      <c r="BK6" t="s">
-        <v>205</v>
       </c>
       <c r="BL6" t="s">
         <v>112</v>
@@ -3103,49 +3100,49 @@
         <v>94</v>
       </c>
       <c r="BQ6" t="s">
+        <v>205</v>
+      </c>
+      <c r="BR6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BS6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>90</v>
+      </c>
+      <c r="BU6" t="s">
+        <v>90</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>94</v>
+      </c>
+      <c r="BW6" t="s">
+        <v>90</v>
+      </c>
+      <c r="BX6" t="s">
+        <v>94</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>90</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>94</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>90</v>
+      </c>
+      <c r="CB6" t="s">
+        <v>90</v>
+      </c>
+      <c r="CC6" t="s">
+        <v>94</v>
+      </c>
+      <c r="CD6" t="s">
         <v>206</v>
       </c>
-      <c r="BR6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BS6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BT6" t="s">
-        <v>90</v>
-      </c>
-      <c r="BU6" t="s">
-        <v>90</v>
-      </c>
-      <c r="BV6" t="s">
-        <v>94</v>
-      </c>
-      <c r="BW6" t="s">
-        <v>90</v>
-      </c>
-      <c r="BX6" t="s">
-        <v>94</v>
-      </c>
-      <c r="BY6" t="s">
-        <v>90</v>
-      </c>
-      <c r="BZ6" t="s">
-        <v>94</v>
-      </c>
-      <c r="CA6" t="s">
-        <v>90</v>
-      </c>
-      <c r="CB6" t="s">
-        <v>90</v>
-      </c>
-      <c r="CC6" t="s">
-        <v>94</v>
-      </c>
-      <c r="CD6" t="s">
+      <c r="CE6" t="s">
         <v>207</v>
-      </c>
-      <c r="CE6" t="s">
-        <v>208</v>
       </c>
       <c r="CF6" t="s">
         <v>94</v>
@@ -3154,36 +3151,36 @@
         <v>118</v>
       </c>
       <c r="CH6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="CI6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="CJ6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="CK6" t="s">
         <v>141</v>
       </c>
       <c r="CL6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="CM6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:95" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" t="s">
         <v>209</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>210</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>211</v>
-      </c>
-      <c r="D7" t="s">
-        <v>212</v>
       </c>
       <c r="E7" t="s">
         <v>89</v>
@@ -3219,16 +3216,16 @@
         <v>94</v>
       </c>
       <c r="Q7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="R7" t="s">
         <v>94</v>
       </c>
       <c r="S7" t="s">
+        <v>212</v>
+      </c>
+      <c r="T7" t="s">
         <v>213</v>
-      </c>
-      <c r="T7" t="s">
-        <v>214</v>
       </c>
       <c r="U7" t="s">
         <v>128</v>
@@ -3237,46 +3234,46 @@
         <v>94</v>
       </c>
       <c r="W7" t="s">
+        <v>214</v>
+      </c>
+      <c r="X7" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF7" t="s">
         <v>215</v>
       </c>
-      <c r="X7" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>216</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>217</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ7" t="s">
         <v>218</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>219</v>
       </c>
       <c r="AK7" t="s">
         <v>94</v>
@@ -3318,10 +3315,10 @@
         <v>94</v>
       </c>
       <c r="AX7" t="s">
+        <v>219</v>
+      </c>
+      <c r="AY7" t="s">
         <v>220</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>221</v>
       </c>
       <c r="AZ7" t="s">
         <v>112</v>
@@ -3330,13 +3327,13 @@
         <v>132</v>
       </c>
       <c r="BB7" t="s">
+        <v>221</v>
+      </c>
+      <c r="BC7" t="s">
         <v>222</v>
       </c>
-      <c r="BC7" t="s">
+      <c r="BD7" t="s">
         <v>223</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>224</v>
       </c>
       <c r="BE7" t="s">
         <v>112</v>
@@ -3348,22 +3345,22 @@
         <v>202</v>
       </c>
       <c r="BH7" t="s">
+        <v>224</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>342</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>94</v>
+      </c>
+      <c r="BK7" t="s">
         <v>225</v>
-      </c>
-      <c r="BI7" t="s">
-        <v>226</v>
-      </c>
-      <c r="BJ7" t="s">
-        <v>94</v>
-      </c>
-      <c r="BK7" t="s">
-        <v>227</v>
       </c>
       <c r="BL7" t="s">
         <v>112</v>
       </c>
       <c r="BM7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="BN7" t="s">
         <v>94</v>
@@ -3372,7 +3369,7 @@
         <v>164</v>
       </c>
       <c r="BP7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BQ7" t="s">
         <v>94</v>
@@ -3411,10 +3408,10 @@
         <v>94</v>
       </c>
       <c r="CD7" t="s">
+        <v>206</v>
+      </c>
+      <c r="CE7" t="s">
         <v>207</v>
-      </c>
-      <c r="CE7" t="s">
-        <v>208</v>
       </c>
       <c r="CF7" t="s">
         <v>94</v>
@@ -3423,48 +3420,48 @@
         <v>118</v>
       </c>
       <c r="CH7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="CI7" t="s">
+        <v>327</v>
+      </c>
+      <c r="CJ7" t="s">
         <v>329</v>
       </c>
-      <c r="CJ7" t="s">
+      <c r="CK7" t="s">
         <v>331</v>
       </c>
-      <c r="CK7" t="s">
-        <v>333</v>
-      </c>
       <c r="CL7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="CM7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="CN7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="CO7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="CP7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="CQ7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:95" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" t="s">
         <v>230</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>231</v>
-      </c>
-      <c r="C8" t="s">
-        <v>232</v>
-      </c>
-      <c r="D8" t="s">
-        <v>233</v>
       </c>
       <c r="E8" t="s">
         <v>89</v>
@@ -3500,67 +3497,67 @@
         <v>94</v>
       </c>
       <c r="P8" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R8" t="s">
+        <v>94</v>
+      </c>
+      <c r="S8" t="s">
+        <v>233</v>
+      </c>
+      <c r="T8" t="s">
         <v>234</v>
       </c>
-      <c r="Q8" t="s">
-        <v>94</v>
-      </c>
-      <c r="R8" t="s">
-        <v>94</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="U8" t="s">
         <v>235</v>
       </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
+        <v>94</v>
+      </c>
+      <c r="W8" t="s">
         <v>236</v>
       </c>
-      <c r="U8" t="s">
+      <c r="X8" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF8" t="s">
         <v>237</v>
       </c>
-      <c r="V8" t="s">
-        <v>94</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="AG8" t="s">
         <v>238</v>
       </c>
-      <c r="X8" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
+        <v>217</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ8" t="s">
         <v>239</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>240</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>218</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>241</v>
       </c>
       <c r="AK8" t="s">
         <v>94</v>
@@ -3602,28 +3599,28 @@
         <v>94</v>
       </c>
       <c r="AX8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>241</v>
+      </c>
+      <c r="AZ8" t="s">
         <v>242</v>
-      </c>
-      <c r="AY8" t="s">
-        <v>243</v>
-      </c>
-      <c r="AZ8" t="s">
-        <v>244</v>
       </c>
       <c r="BA8" t="s">
         <v>108</v>
       </c>
       <c r="BB8" t="s">
+        <v>243</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>244</v>
+      </c>
+      <c r="BD8" t="s">
         <v>245</v>
       </c>
-      <c r="BC8" t="s">
-        <v>246</v>
-      </c>
-      <c r="BD8" t="s">
-        <v>247</v>
-      </c>
       <c r="BE8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="BF8" t="s">
         <v>94</v>
@@ -3656,7 +3653,7 @@
         <v>107</v>
       </c>
       <c r="BP8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="BQ8" t="s">
         <v>94</v>
@@ -3703,16 +3700,16 @@
     </row>
     <row r="9" spans="1:95" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
+        <v>247</v>
+      </c>
+      <c r="B9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" t="s">
         <v>249</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>250</v>
-      </c>
-      <c r="C9" t="s">
-        <v>251</v>
-      </c>
-      <c r="D9" t="s">
-        <v>252</v>
       </c>
       <c r="E9" t="s">
         <v>123</v>
@@ -3748,29 +3745,29 @@
         <v>94</v>
       </c>
       <c r="P9" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>94</v>
+      </c>
+      <c r="R9" t="s">
+        <v>94</v>
+      </c>
+      <c r="S9" t="s">
+        <v>252</v>
+      </c>
+      <c r="T9" t="s">
         <v>253</v>
       </c>
-      <c r="Q9" t="s">
-        <v>94</v>
-      </c>
-      <c r="R9" t="s">
-        <v>94</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="U9" t="s">
         <v>254</v>
       </c>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
         <v>255</v>
       </c>
-      <c r="U9" t="s">
+      <c r="W9" t="s">
         <v>256</v>
       </c>
-      <c r="V9" t="s">
-        <v>257</v>
-      </c>
-      <c r="W9" t="s">
-        <v>258</v>
-      </c>
       <c r="X9" t="s">
         <v>94</v>
       </c>
@@ -3796,19 +3793,19 @@
         <v>94</v>
       </c>
       <c r="AF9" t="s">
+        <v>252</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>253</v>
+      </c>
+      <c r="AH9" t="s">
         <v>254</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AI9" t="s">
         <v>255</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AJ9" t="s">
         <v>256</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>257</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>258</v>
       </c>
       <c r="AK9" t="s">
         <v>94</v>
@@ -3850,28 +3847,28 @@
         <v>94</v>
       </c>
       <c r="AX9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>258</v>
+      </c>
+      <c r="AZ9" t="s">
         <v>259</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>260</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>261</v>
       </c>
       <c r="BA9" t="s">
         <v>132</v>
       </c>
       <c r="BB9" t="s">
+        <v>260</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>261</v>
+      </c>
+      <c r="BD9" t="s">
         <v>262</v>
       </c>
-      <c r="BC9" t="s">
-        <v>263</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>264</v>
-      </c>
       <c r="BE9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="BF9" t="s">
         <v>94</v>
@@ -3907,7 +3904,7 @@
         <v>94</v>
       </c>
       <c r="BQ9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BR9" s="1" t="s">
         <v>94</v>
@@ -3981,16 +3978,16 @@
     </row>
     <row r="10" spans="1:95" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" t="s">
         <v>266</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>267</v>
-      </c>
-      <c r="C10" t="s">
-        <v>268</v>
-      </c>
-      <c r="D10" t="s">
-        <v>269</v>
       </c>
       <c r="E10" t="s">
         <v>123</v>
@@ -4026,67 +4023,67 @@
         <v>94</v>
       </c>
       <c r="P10" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>94</v>
+      </c>
+      <c r="R10" t="s">
+        <v>94</v>
+      </c>
+      <c r="S10" t="s">
+        <v>269</v>
+      </c>
+      <c r="T10" t="s">
         <v>270</v>
       </c>
-      <c r="Q10" t="s">
-        <v>94</v>
-      </c>
-      <c r="R10" t="s">
-        <v>94</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
         <v>271</v>
       </c>
-      <c r="T10" t="s">
+      <c r="V10" t="s">
+        <v>94</v>
+      </c>
+      <c r="W10" t="s">
         <v>272</v>
       </c>
-      <c r="U10" t="s">
+      <c r="X10" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF10" t="s">
         <v>273</v>
       </c>
-      <c r="V10" t="s">
-        <v>94</v>
-      </c>
-      <c r="W10" t="s">
+      <c r="AG10" t="s">
         <v>274</v>
       </c>
-      <c r="X10" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
         <v>275</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AI10" t="s">
         <v>276</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AJ10" t="s">
         <v>277</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>278</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>279</v>
       </c>
       <c r="AK10" t="s">
         <v>94</v>
@@ -4128,64 +4125,64 @@
         <v>94</v>
       </c>
       <c r="AX10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AY10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="AZ10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="BA10" t="s">
         <v>132</v>
       </c>
       <c r="BB10" t="s">
+        <v>280</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>281</v>
+      </c>
+      <c r="BD10" t="s">
         <v>282</v>
       </c>
-      <c r="BC10" t="s">
+      <c r="BE10" t="s">
+        <v>259</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BG10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BN10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BO10" t="s">
+        <v>242</v>
+      </c>
+      <c r="BP10" t="s">
         <v>283</v>
       </c>
-      <c r="BD10" t="s">
+      <c r="BQ10" t="s">
         <v>284</v>
-      </c>
-      <c r="BE10" t="s">
-        <v>261</v>
-      </c>
-      <c r="BF10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BG10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BH10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BI10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BJ10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BK10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BL10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BM10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BN10" t="s">
-        <v>94</v>
-      </c>
-      <c r="BO10" t="s">
-        <v>244</v>
-      </c>
-      <c r="BP10" t="s">
-        <v>285</v>
-      </c>
-      <c r="BQ10" t="s">
-        <v>286</v>
       </c>
       <c r="BR10" s="1" t="s">
         <v>90</v>
@@ -4236,48 +4233,48 @@
         <v>118</v>
       </c>
       <c r="CH10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="CI10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="CJ10" t="s">
+        <v>339</v>
+      </c>
+      <c r="CK10" t="s">
+        <v>328</v>
+      </c>
+      <c r="CL10" t="s">
+        <v>302</v>
+      </c>
+      <c r="CM10" t="s">
         <v>341</v>
       </c>
-      <c r="CK10" t="s">
-        <v>330</v>
-      </c>
-      <c r="CL10" t="s">
-        <v>304</v>
-      </c>
-      <c r="CM10" t="s">
-        <v>343</v>
-      </c>
       <c r="CN10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="CO10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="CP10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="CQ10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:95" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" t="s">
         <v>287</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>288</v>
-      </c>
-      <c r="C11" t="s">
-        <v>289</v>
-      </c>
-      <c r="D11" t="s">
-        <v>290</v>
       </c>
       <c r="E11" t="s">
         <v>89</v>
@@ -4313,29 +4310,29 @@
         <v>94</v>
       </c>
       <c r="P11" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>94</v>
+      </c>
+      <c r="R11" t="s">
+        <v>94</v>
+      </c>
+      <c r="S11" t="s">
+        <v>290</v>
+      </c>
+      <c r="T11" t="s">
         <v>291</v>
       </c>
-      <c r="Q11" t="s">
-        <v>94</v>
-      </c>
-      <c r="R11" t="s">
-        <v>94</v>
-      </c>
-      <c r="S11" t="s">
+      <c r="U11" t="s">
         <v>292</v>
       </c>
-      <c r="T11" t="s">
+      <c r="V11" t="s">
+        <v>94</v>
+      </c>
+      <c r="W11" t="s">
         <v>293</v>
       </c>
-      <c r="U11" t="s">
-        <v>294</v>
-      </c>
-      <c r="V11" t="s">
-        <v>94</v>
-      </c>
-      <c r="W11" t="s">
-        <v>295</v>
-      </c>
       <c r="X11" t="s">
         <v>94</v>
       </c>
@@ -4361,19 +4358,19 @@
         <v>94</v>
       </c>
       <c r="AF11" t="s">
+        <v>290</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>291</v>
+      </c>
+      <c r="AH11" t="s">
         <v>292</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AI11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ11" t="s">
         <v>293</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>294</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>295</v>
       </c>
       <c r="AK11" t="s">
         <v>94</v>
@@ -4415,28 +4412,28 @@
         <v>94</v>
       </c>
       <c r="AX11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AY11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AZ11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="BA11" t="s">
         <v>132</v>
       </c>
       <c r="BB11" t="s">
+        <v>296</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>297</v>
+      </c>
+      <c r="BD11" t="s">
         <v>298</v>
       </c>
-      <c r="BC11" t="s">
-        <v>299</v>
-      </c>
-      <c r="BD11" t="s">
-        <v>300</v>
-      </c>
       <c r="BE11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="BF11" t="s">
         <v>94</v>
@@ -4445,22 +4442,22 @@
         <v>136</v>
       </c>
       <c r="BH11" t="s">
+        <v>299</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>94</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>300</v>
+      </c>
+      <c r="BK11" t="s">
         <v>301</v>
-      </c>
-      <c r="BI11" t="s">
-        <v>94</v>
-      </c>
-      <c r="BJ11" t="s">
-        <v>302</v>
-      </c>
-      <c r="BK11" t="s">
-        <v>303</v>
       </c>
       <c r="BL11" t="s">
         <v>140</v>
       </c>
       <c r="BM11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BN11" t="s">
         <v>94</v>
@@ -4472,7 +4469,7 @@
         <v>94</v>
       </c>
       <c r="BQ11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="BR11" s="1" t="s">
         <v>94</v>
@@ -4526,7 +4523,7 @@
         <v>94</v>
       </c>
       <c r="CI11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="CJ11" t="s">
         <v>94</v>
@@ -4555,16 +4552,16 @@
     </row>
     <row r="12" spans="1:95" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" t="s">
         <v>309</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="C12" t="s">
-        <v>311</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="E12" t="s">
         <v>89</v>
@@ -4600,52 +4597,70 @@
         <v>94</v>
       </c>
       <c r="P12" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>94</v>
+      </c>
+      <c r="S12" t="s">
+        <v>311</v>
+      </c>
+      <c r="T12" t="s">
+        <v>313</v>
+      </c>
+      <c r="U12" t="s">
         <v>314</v>
       </c>
-      <c r="Q12" t="s">
-        <v>94</v>
-      </c>
-      <c r="S12" t="s">
+      <c r="W12" t="s">
+        <v>315</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG12" t="s">
         <v>313</v>
       </c>
-      <c r="T12" t="s">
+      <c r="AH12" t="s">
+        <v>314</v>
+      </c>
+      <c r="AJ12" t="s">
         <v>315</v>
       </c>
-      <c r="U12" t="s">
-        <v>316</v>
-      </c>
-      <c r="W12" t="s">
-        <v>317</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>313</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>315</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>316</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>317</v>
+      <c r="AR12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>104</v>
+      </c>
+      <c r="BO12" t="s">
+        <v>112</v>
       </c>
       <c r="CH12" t="s">
+        <v>334</v>
+      </c>
+      <c r="CI12" t="s">
+        <v>327</v>
+      </c>
+      <c r="CJ12" t="s">
+        <v>337</v>
+      </c>
+      <c r="CK12" t="s">
+        <v>226</v>
+      </c>
+      <c r="CL12" t="s">
+        <v>326</v>
+      </c>
+      <c r="CM12" t="s">
         <v>336</v>
-      </c>
-      <c r="CI12" t="s">
-        <v>329</v>
-      </c>
-      <c r="CJ12" t="s">
-        <v>339</v>
-      </c>
-      <c r="CK12" t="s">
-        <v>228</v>
-      </c>
-      <c r="CL12" t="s">
-        <v>328</v>
-      </c>
-      <c r="CM12" t="s">
-        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maybe fixed test errors, not sure
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aholmes/Developer/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashankland/git/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF8A2B8-BBB5-D743-81DE-DE59819AC946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F1F2CC-B994-3B43-9F93-B0B115DDC40F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="450">
   <si>
     <t>First Name</t>
   </si>
@@ -1361,6 +1361,15 @@
   </si>
   <si>
     <t>Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Race Unknown</t>
+  </si>
+  <si>
+    <t>Race Other</t>
+  </si>
+  <si>
+    <t>Race Refused to Answer</t>
   </si>
 </sst>
 </file>
@@ -1713,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU12"/>
+  <dimension ref="A1:CX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CK1" workbookViewId="0">
-      <selection activeCell="CU2" sqref="CU2"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="M13" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1731,96 +1740,97 @@
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="35" customWidth="1"/>
+    <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.5" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="29" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="30" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="20" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="30" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="24" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="38" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="16" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="12" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="29" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="30" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="24" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="20" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="30" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="24" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="38" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="16" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="12" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="12" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1852,274 +1862,283 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>447</v>
+      </c>
+      <c r="L1" t="s">
+        <v>448</v>
+      </c>
+      <c r="M1" t="s">
+        <v>449</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BI1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BK1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BL1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BM1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BN1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BO1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BP1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BQ1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BR1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BS1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BT1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BW1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BX1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BY1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BZ1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CA1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CB1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CC1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CD1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CE1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CF1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CG1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CH1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CI1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CJ1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CK1" t="s">
         <v>301</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CL1" t="s">
         <v>302</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CM1" t="s">
         <v>303</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CN1" t="s">
         <v>304</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CO1" t="s">
         <v>305</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CP1" t="s">
         <v>306</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CQ1" t="s">
         <v>307</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CR1" t="s">
         <v>308</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CS1" t="s">
         <v>309</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CT1" t="s">
         <v>310</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CU1" t="s">
         <v>388</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CV1" t="s">
         <v>387</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CW1" t="s">
         <v>445</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CX1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2150,54 +2169,54 @@
       <c r="J2" t="s">
         <v>89</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
         <v>391</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>92</v>
       </c>
-      <c r="M2" t="s">
-        <v>93</v>
-      </c>
-      <c r="N2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O2" t="s">
-        <v>93</v>
-      </c>
       <c r="P2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" t="s">
+        <v>93</v>
+      </c>
+      <c r="S2" t="s">
         <v>94</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>290</v>
       </c>
-      <c r="R2" t="s">
-        <v>93</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
+        <v>93</v>
+      </c>
+      <c r="V2" t="s">
         <v>95</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>96</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>97</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>98</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>99</v>
       </c>
-      <c r="X2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>93</v>
-      </c>
       <c r="AA2" t="s">
         <v>93</v>
       </c>
@@ -2214,29 +2233,29 @@
         <v>93</v>
       </c>
       <c r="AF2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI2" t="s">
         <v>95</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AJ2" t="s">
         <v>96</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AK2" t="s">
         <v>97</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AL2" t="s">
         <v>98</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AM2" t="s">
         <v>99</v>
       </c>
-      <c r="AK2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>93</v>
-      </c>
       <c r="AN2" t="s">
         <v>93</v>
       </c>
@@ -2250,62 +2269,62 @@
         <v>93</v>
       </c>
       <c r="AR2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU2" t="s">
         <v>396</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AV2" t="s">
         <v>101</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AW2" t="s">
         <v>402</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AX2" t="s">
         <v>101</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AY2" t="s">
         <v>103</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AZ2" t="s">
         <v>417</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BA2" t="s">
         <v>104</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BB2" t="s">
         <v>105</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BC2" t="s">
         <v>106</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BD2" t="s">
         <v>107</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BE2" t="s">
         <v>108</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BF2" t="s">
         <v>109</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BG2" t="s">
         <v>110</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BH2" t="s">
         <v>111</v>
       </c>
-      <c r="BF2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG2" t="s">
+      <c r="BI2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ2" t="s">
         <v>422</v>
       </c>
-      <c r="BH2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>93</v>
-      </c>
       <c r="BK2" t="s">
         <v>93</v>
       </c>
@@ -2319,43 +2338,43 @@
         <v>93</v>
       </c>
       <c r="BO2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR2" t="s">
         <v>112</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BS2" t="s">
         <v>113</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BT2" t="s">
         <v>114</v>
       </c>
-      <c r="BR2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BS2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>89</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>89</v>
-      </c>
-      <c r="BV2" t="s">
+      <c r="BU2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BV2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="BW2" t="s">
         <v>89</v>
       </c>
       <c r="BX2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="BY2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="BZ2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="CA2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="CB2" t="s">
         <v>89</v>
@@ -2364,21 +2383,21 @@
         <v>93</v>
       </c>
       <c r="CD2" t="s">
+        <v>89</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>89</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG2" t="s">
         <v>115</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CH2" t="s">
         <v>432</v>
       </c>
-      <c r="CF2" t="s">
-        <v>93</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>93</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>93</v>
-      </c>
-      <c r="CL2" t="s">
+      <c r="CI2" t="s">
         <v>93</v>
       </c>
       <c r="CM2" t="s">
@@ -2396,11 +2415,20 @@
       <c r="CQ2" t="s">
         <v>93</v>
       </c>
-      <c r="CS2">
+      <c r="CR2" t="s">
+        <v>93</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>93</v>
+      </c>
+      <c r="CV2">
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2431,57 +2459,57 @@
       <c r="J3" t="s">
         <v>89</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
         <v>389</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>92</v>
       </c>
-      <c r="M3" t="s">
-        <v>93</v>
-      </c>
-      <c r="N3" t="s">
-        <v>89</v>
-      </c>
-      <c r="O3" t="s">
-        <v>93</v>
-      </c>
       <c r="P3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R3" t="s">
+        <v>93</v>
+      </c>
+      <c r="S3" t="s">
         <v>122</v>
       </c>
-      <c r="Q3" t="s">
-        <v>93</v>
-      </c>
-      <c r="R3" t="s">
-        <v>93</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
+        <v>93</v>
+      </c>
+      <c r="U3" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" t="s">
         <v>123</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
         <v>124</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>125</v>
       </c>
-      <c r="V3" t="s">
-        <v>93</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z3" t="s">
         <v>126</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>358</v>
       </c>
-      <c r="Z3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>93</v>
-      </c>
       <c r="AC3" t="s">
         <v>93</v>
       </c>
@@ -2492,29 +2520,29 @@
         <v>93</v>
       </c>
       <c r="AF3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI3" t="s">
         <v>123</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AJ3" t="s">
         <v>124</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AK3" t="s">
         <v>125</v>
       </c>
-      <c r="AI3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AJ3" t="s">
+      <c r="AL3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM3" t="s">
         <v>126</v>
       </c>
-      <c r="AK3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>93</v>
-      </c>
       <c r="AN3" t="s">
         <v>93</v>
       </c>
@@ -2528,163 +2556,172 @@
         <v>93</v>
       </c>
       <c r="AR3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU3" t="s">
         <v>369</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AV3" t="s">
         <v>101</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AW3" t="s">
         <v>403</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AX3" t="s">
         <v>101</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AY3" t="s">
         <v>415</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AZ3" t="s">
         <v>416</v>
       </c>
-      <c r="AX3" t="s">
+      <c r="BA3" t="s">
         <v>127</v>
       </c>
-      <c r="AY3" t="s">
+      <c r="BB3" t="s">
         <v>128</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BC3" t="s">
         <v>111</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BD3" t="s">
         <v>129</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BE3" t="s">
         <v>130</v>
       </c>
-      <c r="BC3" t="s">
+      <c r="BF3" t="s">
         <v>131</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BG3" t="s">
         <v>132</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BH3" t="s">
         <v>111</v>
       </c>
-      <c r="BF3" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG3" t="s">
+      <c r="BI3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ3" t="s">
         <v>133</v>
       </c>
-      <c r="BH3" t="s">
+      <c r="BK3" t="s">
         <v>134</v>
       </c>
-      <c r="BI3" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ3" t="s">
+      <c r="BL3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM3" t="s">
         <v>135</v>
       </c>
-      <c r="BK3" t="s">
+      <c r="BN3" t="s">
         <v>136</v>
       </c>
-      <c r="BL3" t="s">
+      <c r="BO3" t="s">
         <v>137</v>
       </c>
-      <c r="BM3" t="s">
+      <c r="BP3" t="s">
         <v>138</v>
       </c>
-      <c r="BN3" t="s">
-        <v>93</v>
-      </c>
-      <c r="BO3" t="s">
+      <c r="BQ3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR3" t="s">
         <v>112</v>
       </c>
-      <c r="BP3" t="s">
-        <v>93</v>
-      </c>
-      <c r="BQ3" t="s">
+      <c r="BS3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BT3" t="s">
         <v>139</v>
       </c>
-      <c r="BR3" s="1" t="s">
+      <c r="BU3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BS3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BT3" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="BU3" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="BV3" t="s">
+      <c r="BV3" s="1" t="s">
         <v>93</v>
       </c>
       <c r="BW3" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="BX3" t="s">
-        <v>93</v>
+      <c r="BX3" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="BY3" t="s">
-        <v>89</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>93</v>
+        <v>93</v>
+      </c>
+      <c r="BZ3" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="CA3" t="s">
-        <v>89</v>
-      </c>
-      <c r="CB3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>89</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>89</v>
+      </c>
+      <c r="CE3" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="CC3" t="s">
-        <v>93</v>
-      </c>
-      <c r="CD3" t="s">
+      <c r="CF3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG3" t="s">
         <v>140</v>
       </c>
-      <c r="CE3" t="s">
+      <c r="CH3" t="s">
         <v>433</v>
       </c>
-      <c r="CF3" t="s">
+      <c r="CI3" t="s">
         <v>333</v>
       </c>
-      <c r="CG3" t="s">
+      <c r="CJ3" t="s">
         <v>117</v>
       </c>
-      <c r="CH3" t="s">
+      <c r="CK3" t="s">
         <v>313</v>
       </c>
-      <c r="CI3" t="s">
+      <c r="CL3" t="s">
         <v>312</v>
       </c>
-      <c r="CJ3" t="s">
+      <c r="CM3" t="s">
         <v>314</v>
       </c>
-      <c r="CK3" t="s">
+      <c r="CN3" t="s">
         <v>315</v>
       </c>
-      <c r="CL3" t="s">
+      <c r="CO3" t="s">
         <v>316</v>
       </c>
-      <c r="CM3" t="s">
+      <c r="CP3" t="s">
         <v>317</v>
       </c>
-      <c r="CN3" t="s">
-        <v>93</v>
-      </c>
-      <c r="CO3" t="s">
-        <v>93</v>
-      </c>
-      <c r="CP3" t="s">
-        <v>93</v>
-      </c>
       <c r="CQ3" t="s">
         <v>93</v>
       </c>
+      <c r="CR3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -2715,51 +2752,51 @@
       <c r="J4" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" t="s">
         <v>390</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>92</v>
       </c>
-      <c r="M4" t="s">
-        <v>93</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="O4" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>93</v>
-      </c>
       <c r="R4" t="s">
         <v>93</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
+        <v>93</v>
+      </c>
+      <c r="U4" t="s">
+        <v>93</v>
+      </c>
+      <c r="V4" t="s">
         <v>145</v>
       </c>
-      <c r="T4" t="s">
+      <c r="W4" t="s">
         <v>146</v>
       </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
         <v>147</v>
       </c>
-      <c r="V4" t="s">
-        <v>93</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z4" t="s">
         <v>148</v>
       </c>
-      <c r="X4" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>93</v>
-      </c>
       <c r="AA4" t="s">
         <v>93</v>
       </c>
@@ -2776,32 +2813,32 @@
         <v>93</v>
       </c>
       <c r="AF4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI4" t="s">
         <v>149</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AJ4" t="s">
         <v>150</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AK4" t="s">
         <v>368</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AL4" t="s">
         <v>152</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AM4" t="s">
         <v>153</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AN4" t="s">
         <v>376</v>
       </c>
-      <c r="AL4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>93</v>
-      </c>
       <c r="AO4" t="s">
         <v>93</v>
       </c>
@@ -2812,62 +2849,62 @@
         <v>93</v>
       </c>
       <c r="AR4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU4" t="s">
         <v>100</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AV4" t="s">
         <v>101</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AW4" t="s">
         <v>154</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AX4" t="s">
         <v>101</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AY4" t="s">
         <v>410</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AZ4" t="s">
         <v>418</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="BA4" t="s">
         <v>155</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="BB4" t="s">
         <v>156</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BC4" t="s">
         <v>111</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BD4" t="s">
         <v>129</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BE4" t="s">
         <v>157</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BF4" t="s">
         <v>158</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BG4" t="s">
         <v>159</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BH4" t="s">
         <v>111</v>
       </c>
-      <c r="BF4" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG4" t="s">
+      <c r="BI4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ4" t="s">
         <v>423</v>
       </c>
-      <c r="BH4" t="s">
-        <v>93</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>93</v>
-      </c>
       <c r="BK4" t="s">
         <v>93</v>
       </c>
@@ -2878,97 +2915,106 @@
         <v>93</v>
       </c>
       <c r="BN4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>352</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="BR4" t="s">
         <v>160</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="BS4" t="s">
         <v>161</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="BT4" t="s">
         <v>162</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="BT4" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="BU4" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="BV4" t="s">
-        <v>93</v>
       </c>
       <c r="BW4" s="1" t="s">
         <v>326</v>
       </c>
       <c r="BX4" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BZ4" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="CA4" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="BY4" s="1" t="s">
+      <c r="CB4" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CC4" t="s">
         <v>341</v>
       </c>
-      <c r="CA4" s="1" t="s">
+      <c r="CD4" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CE4" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="CC4" t="s">
-        <v>93</v>
-      </c>
-      <c r="CD4" s="1" t="s">
+      <c r="CF4" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG4" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CH4" t="s">
         <v>141</v>
       </c>
-      <c r="CF4" t="s">
-        <v>93</v>
-      </c>
-      <c r="CG4" t="s">
+      <c r="CI4" t="s">
+        <v>93</v>
+      </c>
+      <c r="CJ4" t="s">
         <v>117</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CK4" t="s">
         <v>288</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CL4" t="s">
         <v>439</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CM4" t="s">
         <v>314</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CN4" t="s">
         <v>318</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CO4" t="s">
         <v>319</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CP4" t="s">
         <v>317</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CQ4" t="s">
         <v>314</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CR4" t="s">
         <v>214</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CS4" t="s">
         <v>316</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CT4" t="s">
         <v>320</v>
       </c>
-      <c r="CS4">
+      <c r="CV4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -2999,54 +3045,54 @@
       <c r="J5" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" t="s">
         <v>91</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>92</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="O5" t="s">
-        <v>93</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
+        <v>93</v>
+      </c>
+      <c r="S5" t="s">
         <v>167</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>291</v>
       </c>
-      <c r="R5" t="s">
-        <v>93</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
+        <v>93</v>
+      </c>
+      <c r="V5" t="s">
         <v>168</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" t="s">
         <v>169</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>328</v>
       </c>
-      <c r="V5" t="s">
-        <v>93</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z5" t="s">
         <v>171</v>
       </c>
-      <c r="X5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>93</v>
-      </c>
       <c r="AA5" t="s">
         <v>93</v>
       </c>
@@ -3063,32 +3109,32 @@
         <v>93</v>
       </c>
       <c r="AF5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI5" t="s">
         <v>168</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AJ5" t="s">
         <v>169</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AK5" t="s">
         <v>170</v>
       </c>
-      <c r="AI5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AJ5" t="s">
+      <c r="AL5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM5" t="s">
         <v>171</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AN5" t="s">
         <v>377</v>
       </c>
-      <c r="AL5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>93</v>
-      </c>
       <c r="AO5" t="s">
         <v>93</v>
       </c>
@@ -3099,41 +3145,41 @@
         <v>93</v>
       </c>
       <c r="AR5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU5" t="s">
         <v>401</v>
       </c>
-      <c r="AS5">
+      <c r="AV5">
         <v>3333333333</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AW5" t="s">
         <v>408</v>
       </c>
-      <c r="AU5">
+      <c r="AX5">
         <v>3333333333</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AY5" t="s">
         <v>103</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AZ5" t="s">
         <v>354</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="BA5" t="s">
         <v>172</v>
       </c>
-      <c r="BF5" t="s">
+      <c r="BI5" t="s">
         <v>378</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="BJ5" t="s">
         <v>424</v>
       </c>
-      <c r="BI5" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>93</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>93</v>
-      </c>
       <c r="BL5" t="s">
         <v>93</v>
       </c>
@@ -3144,70 +3190,79 @@
         <v>93</v>
       </c>
       <c r="BO5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR5" t="s">
         <v>173</v>
       </c>
-      <c r="BP5" t="s">
+      <c r="BS5" t="s">
         <v>174</v>
       </c>
-      <c r="BQ5" t="s">
+      <c r="BT5" t="s">
         <v>175</v>
       </c>
-      <c r="BR5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BS5" s="1" t="s">
+      <c r="BU5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BV5" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="BT5" t="b">
-        <v>0</v>
-      </c>
-      <c r="BU5" t="b">
-        <v>0</v>
-      </c>
-      <c r="BV5" t="s">
-        <v>347</v>
       </c>
       <c r="BW5" t="b">
         <v>0</v>
       </c>
-      <c r="BX5" t="s">
-        <v>93</v>
-      </c>
-      <c r="BY5" s="1" t="s">
+      <c r="BX5" t="b">
+        <v>0</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>347</v>
+      </c>
+      <c r="BZ5" t="b">
+        <v>0</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB5" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="BZ5" t="s">
-        <v>93</v>
-      </c>
-      <c r="CA5" s="1" t="s">
+      <c r="CC5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CD5" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="CB5" t="b">
+      <c r="CE5" t="b">
         <v>0</v>
       </c>
-      <c r="CC5" t="s">
+      <c r="CF5" t="s">
         <v>338</v>
       </c>
-      <c r="CD5" s="1" t="s">
+      <c r="CG5" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="CE5" t="s">
+      <c r="CH5" t="s">
         <v>116</v>
       </c>
-      <c r="CF5" t="s">
-        <v>93</v>
-      </c>
-      <c r="CH5" s="2">
+      <c r="CI5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CK5" s="2">
         <v>43953</v>
       </c>
-      <c r="CI5" t="s">
+      <c r="CL5" t="s">
         <v>440</v>
       </c>
-      <c r="CS5">
+      <c r="CV5">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3238,230 +3293,239 @@
       <c r="J6" t="b">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
         <v>394</v>
       </c>
-      <c r="L6" t="s">
+      <c r="O6" t="s">
         <v>92</v>
       </c>
-      <c r="M6" t="s">
-        <v>93</v>
-      </c>
-      <c r="N6" t="b">
+      <c r="P6" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q6" t="b">
         <v>0</v>
       </c>
-      <c r="O6" t="s">
-        <v>93</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
+        <v>93</v>
+      </c>
+      <c r="S6" t="s">
         <v>180</v>
       </c>
-      <c r="Q6" t="s">
-        <v>93</v>
-      </c>
-      <c r="R6" t="s">
-        <v>93</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
+        <v>93</v>
+      </c>
+      <c r="U6" t="s">
+        <v>93</v>
+      </c>
+      <c r="V6" t="s">
         <v>181</v>
       </c>
-      <c r="T6" t="s">
+      <c r="W6" t="s">
         <v>182</v>
       </c>
-      <c r="U6" t="s">
+      <c r="X6" t="s">
         <v>383</v>
       </c>
-      <c r="W6">
+      <c r="Z6">
         <v>76434</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AB6" t="s">
         <v>181</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AC6" t="s">
         <v>182</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AD6" t="s">
         <v>359</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AE6" t="s">
         <v>364</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AF6" t="s">
         <v>183</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AG6" t="s">
         <v>365</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AH6" t="s">
         <v>361</v>
       </c>
-      <c r="AK6" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL6" t="s">
+      <c r="AN6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO6" t="s">
         <v>184</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AP6" t="s">
         <v>185</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AQ6" t="s">
         <v>367</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AR6" t="s">
         <v>374</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AS6" t="s">
         <v>186</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AT6" t="s">
         <v>372</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AU6" t="s">
         <v>396</v>
       </c>
-      <c r="AS6" s="1" t="s">
+      <c r="AV6" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AW6" t="s">
         <v>404</v>
       </c>
-      <c r="AU6" s="1" t="s">
+      <c r="AX6" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AY6" t="s">
         <v>103</v>
       </c>
-      <c r="AW6" s="1" t="s">
+      <c r="AZ6" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="BA6" t="s">
         <v>187</v>
       </c>
-      <c r="AY6" t="s">
+      <c r="BB6" t="s">
         <v>188</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="BC6" t="s">
         <v>106</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BD6" t="s">
         <v>107</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="BE6" t="s">
         <v>189</v>
       </c>
-      <c r="BC6" t="s">
+      <c r="BF6" t="s">
         <v>190</v>
       </c>
-      <c r="BD6" t="s">
+      <c r="BG6" t="s">
         <v>191</v>
       </c>
-      <c r="BE6" t="s">
+      <c r="BH6" t="s">
         <v>111</v>
       </c>
-      <c r="BF6" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG6" t="s">
+      <c r="BI6" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ6" t="s">
         <v>192</v>
       </c>
-      <c r="BH6" t="s">
+      <c r="BK6" t="s">
         <v>193</v>
       </c>
-      <c r="BI6" t="s">
+      <c r="BL6" t="s">
         <v>151</v>
       </c>
-      <c r="BJ6" t="s">
-        <v>93</v>
-      </c>
-      <c r="BK6" t="s">
+      <c r="BM6" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN6" t="s">
         <v>194</v>
       </c>
-      <c r="BL6" t="s">
+      <c r="BO6" t="s">
         <v>111</v>
       </c>
-      <c r="BM6" t="s">
+      <c r="BP6" t="s">
         <v>111</v>
       </c>
-      <c r="BN6" t="s">
-        <v>93</v>
-      </c>
-      <c r="BO6" t="s">
+      <c r="BQ6" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR6" t="s">
         <v>173</v>
       </c>
-      <c r="BP6" t="s">
-        <v>93</v>
-      </c>
-      <c r="BQ6" t="s">
+      <c r="BS6" t="s">
+        <v>93</v>
+      </c>
+      <c r="BT6" t="s">
         <v>195</v>
       </c>
-      <c r="BR6" s="1" t="s">
+      <c r="BU6" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="BS6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BT6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BU6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BV6" t="s">
+      <c r="BV6" s="1" t="s">
         <v>93</v>
       </c>
       <c r="BW6" t="b">
         <v>1</v>
       </c>
-      <c r="BX6" t="s">
-        <v>93</v>
-      </c>
-      <c r="BY6" t="b">
+      <c r="BX6" t="b">
+        <v>1</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>93</v>
+      </c>
+      <c r="BZ6" t="b">
+        <v>1</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB6" t="b">
         <v>0</v>
       </c>
-      <c r="BZ6" t="s">
+      <c r="CC6" t="s">
         <v>340</v>
       </c>
-      <c r="CA6" t="b">
+      <c r="CD6" t="b">
         <v>0</v>
       </c>
-      <c r="CB6" t="b">
+      <c r="CE6" t="b">
         <v>1</v>
       </c>
-      <c r="CC6" t="s">
-        <v>93</v>
-      </c>
-      <c r="CE6" t="s">
+      <c r="CF6" t="s">
+        <v>93</v>
+      </c>
+      <c r="CH6" t="s">
         <v>196</v>
       </c>
-      <c r="CF6" t="s">
+      <c r="CI6" t="s">
         <v>334</v>
       </c>
-      <c r="CG6" t="s">
+      <c r="CJ6" t="s">
         <v>117</v>
       </c>
-      <c r="CH6" t="s">
+      <c r="CK6" t="s">
         <v>323</v>
       </c>
-      <c r="CI6" t="s">
+      <c r="CL6" t="s">
         <v>441</v>
       </c>
-      <c r="CJ6" t="s">
+      <c r="CM6" t="s">
         <v>324</v>
       </c>
-      <c r="CK6" s="2">
+      <c r="CN6" s="2">
         <v>43953</v>
       </c>
-      <c r="CL6" s="3">
+      <c r="CO6" s="3">
         <v>43962</v>
       </c>
-      <c r="CM6" t="s">
+      <c r="CP6" t="s">
         <v>325</v>
       </c>
-      <c r="CS6">
+      <c r="CV6">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3492,236 +3556,245 @@
       <c r="J7" t="b">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
         <v>91</v>
       </c>
-      <c r="L7" t="s">
+      <c r="O7" t="s">
         <v>92</v>
       </c>
-      <c r="M7" t="s">
-        <v>93</v>
-      </c>
-      <c r="N7" t="b">
+      <c r="P7" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q7" t="b">
         <v>1</v>
       </c>
-      <c r="O7" t="s">
+      <c r="R7" t="s">
         <v>380</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
         <v>292</v>
       </c>
-      <c r="R7" t="s">
-        <v>93</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
+        <v>93</v>
+      </c>
+      <c r="V7" t="s">
         <v>200</v>
       </c>
-      <c r="T7" t="s">
+      <c r="W7" t="s">
         <v>201</v>
       </c>
-      <c r="U7" t="s">
+      <c r="X7" t="s">
         <v>384</v>
       </c>
-      <c r="W7">
+      <c r="Z7">
         <v>42123</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AB7" t="s">
         <v>200</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AC7" t="s">
         <v>201</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AD7" t="s">
         <v>360</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AE7" t="s">
         <v>363</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AF7" t="s">
         <v>202</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AG7" t="s">
         <v>362</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AH7" t="s">
         <v>366</v>
       </c>
-      <c r="AK7" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL7" t="s">
+      <c r="AN7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO7" t="s">
         <v>203</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AP7" t="s">
         <v>204</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AQ7" t="s">
         <v>205</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AR7" t="s">
         <v>375</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AS7" t="s">
         <v>206</v>
       </c>
-      <c r="AQ7" t="s">
+      <c r="AT7" t="s">
         <v>373</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AU7" t="s">
         <v>397</v>
       </c>
-      <c r="AS7">
+      <c r="AV7">
         <v>3333333333</v>
       </c>
-      <c r="AT7" t="s">
+      <c r="AW7" t="s">
         <v>405</v>
       </c>
-      <c r="AU7">
+      <c r="AX7">
         <v>3333333333</v>
       </c>
-      <c r="AV7" t="s">
+      <c r="AY7" t="s">
         <v>411</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AZ7" t="s">
         <v>355</v>
       </c>
-      <c r="AX7" t="s">
+      <c r="BA7" t="s">
         <v>207</v>
       </c>
-      <c r="AY7" t="s">
+      <c r="BB7" t="s">
         <v>208</v>
       </c>
-      <c r="AZ7" t="s">
+      <c r="BC7" t="s">
         <v>111</v>
       </c>
-      <c r="BA7" t="s">
+      <c r="BD7" t="s">
         <v>129</v>
       </c>
-      <c r="BB7" t="s">
+      <c r="BE7" t="s">
         <v>209</v>
       </c>
-      <c r="BC7" t="s">
+      <c r="BF7" t="s">
         <v>210</v>
       </c>
-      <c r="BD7" t="s">
+      <c r="BG7" t="s">
         <v>211</v>
       </c>
-      <c r="BE7" t="s">
+      <c r="BH7" t="s">
         <v>111</v>
       </c>
-      <c r="BF7" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG7" t="s">
+      <c r="BI7" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ7" t="s">
         <v>426</v>
       </c>
-      <c r="BH7" t="s">
+      <c r="BK7" t="s">
         <v>212</v>
       </c>
-      <c r="BI7" t="s">
+      <c r="BL7" t="s">
         <v>332</v>
       </c>
-      <c r="BJ7" t="s">
-        <v>93</v>
-      </c>
-      <c r="BK7" t="s">
+      <c r="BM7" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN7" t="s">
         <v>213</v>
       </c>
-      <c r="BL7" s="2">
+      <c r="BO7" s="2">
         <v>43946</v>
       </c>
-      <c r="BM7" s="2">
+      <c r="BP7" s="2">
         <v>43951</v>
       </c>
-      <c r="BN7" t="s">
-        <v>93</v>
-      </c>
-      <c r="BO7" s="2">
+      <c r="BQ7" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR7" s="2">
         <v>43943</v>
       </c>
-      <c r="BP7" t="s">
+      <c r="BS7" t="s">
         <v>215</v>
       </c>
-      <c r="BQ7" t="s">
-        <v>93</v>
-      </c>
-      <c r="BR7" s="1" t="s">
+      <c r="BT7" t="s">
+        <v>93</v>
+      </c>
+      <c r="BU7" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="BT7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BU7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BV7" t="s">
-        <v>93</v>
       </c>
       <c r="BW7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BX7" t="s">
-        <v>93</v>
-      </c>
-      <c r="BY7" t="b">
+      <c r="BX7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>93</v>
+      </c>
+      <c r="BZ7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CA7" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB7" t="b">
         <v>1</v>
       </c>
-      <c r="BZ7" t="s">
-        <v>93</v>
-      </c>
-      <c r="CA7" t="b">
+      <c r="CC7" t="s">
+        <v>93</v>
+      </c>
+      <c r="CD7" t="b">
         <v>1</v>
       </c>
-      <c r="CB7" s="1" t="s">
+      <c r="CE7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CC7" t="s">
+      <c r="CF7" t="s">
         <v>337</v>
       </c>
-      <c r="CD7" t="s">
+      <c r="CG7" t="s">
         <v>429</v>
       </c>
-      <c r="CE7" t="s">
+      <c r="CH7" t="s">
         <v>434</v>
       </c>
-      <c r="CF7" t="s">
-        <v>93</v>
-      </c>
-      <c r="CG7" t="s">
+      <c r="CI7" t="s">
+        <v>93</v>
+      </c>
+      <c r="CJ7" t="s">
         <v>117</v>
       </c>
-      <c r="CH7" s="3">
+      <c r="CK7" s="3">
         <v>43954</v>
       </c>
-      <c r="CI7" t="s">
+      <c r="CL7" t="s">
         <v>312</v>
       </c>
-      <c r="CJ7" t="s">
+      <c r="CM7" t="s">
         <v>314</v>
       </c>
-      <c r="CK7" t="s">
+      <c r="CN7" t="s">
         <v>316</v>
       </c>
-      <c r="CL7" t="s">
+      <c r="CO7" t="s">
         <v>288</v>
       </c>
-      <c r="CM7" t="s">
+      <c r="CP7" t="s">
         <v>325</v>
       </c>
-      <c r="CN7" t="s">
+      <c r="CQ7" t="s">
         <v>322</v>
       </c>
-      <c r="CO7" s="2">
+      <c r="CR7" s="2">
         <v>43954</v>
       </c>
-      <c r="CP7" s="3">
+      <c r="CS7" s="3">
         <v>43955</v>
       </c>
-      <c r="CQ7" t="s">
+      <c r="CT7" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3752,54 +3825,54 @@
       <c r="J8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N8" t="s">
         <v>392</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>92</v>
       </c>
-      <c r="M8" t="s">
-        <v>93</v>
-      </c>
-      <c r="N8" s="1" t="s">
+      <c r="P8" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O8" t="s">
-        <v>93</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
+        <v>93</v>
+      </c>
+      <c r="S8" t="s">
         <v>220</v>
       </c>
-      <c r="Q8" t="s">
-        <v>93</v>
-      </c>
-      <c r="R8">
+      <c r="T8" t="s">
+        <v>93</v>
+      </c>
+      <c r="U8">
         <v>24872138</v>
       </c>
-      <c r="S8" t="s">
+      <c r="V8" t="s">
         <v>221</v>
       </c>
-      <c r="T8" t="s">
+      <c r="W8" t="s">
         <v>222</v>
       </c>
-      <c r="U8" t="s">
+      <c r="X8" t="s">
         <v>223</v>
       </c>
-      <c r="V8" t="s">
-        <v>93</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="Y8" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z8" t="s">
         <v>224</v>
       </c>
-      <c r="X8" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>93</v>
-      </c>
       <c r="AA8" t="s">
         <v>93</v>
       </c>
@@ -3816,29 +3889,29 @@
         <v>93</v>
       </c>
       <c r="AF8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI8" t="s">
         <v>225</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AJ8" t="s">
         <v>226</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AK8" t="s">
         <v>205</v>
       </c>
-      <c r="AI8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AJ8" t="s">
+      <c r="AL8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM8" t="s">
         <v>227</v>
       </c>
-      <c r="AK8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>93</v>
-      </c>
       <c r="AN8" t="s">
         <v>93</v>
       </c>
@@ -3852,62 +3925,62 @@
         <v>93</v>
       </c>
       <c r="AR8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU8" t="s">
         <v>370</v>
       </c>
-      <c r="AS8">
+      <c r="AV8">
         <v>13333333333</v>
       </c>
-      <c r="AT8" t="s">
+      <c r="AW8" t="s">
         <v>406</v>
       </c>
-      <c r="AU8">
+      <c r="AX8">
         <v>13333333333</v>
       </c>
-      <c r="AV8" t="s">
+      <c r="AY8" t="s">
         <v>103</v>
       </c>
-      <c r="AW8" t="s">
+      <c r="AZ8" t="s">
         <v>420</v>
       </c>
-      <c r="AX8" t="s">
+      <c r="BA8" t="s">
         <v>228</v>
       </c>
-      <c r="AY8" t="s">
+      <c r="BB8" t="s">
         <v>229</v>
       </c>
-      <c r="AZ8" t="s">
+      <c r="BC8" t="s">
         <v>230</v>
       </c>
-      <c r="BA8" t="s">
+      <c r="BD8" t="s">
         <v>107</v>
       </c>
-      <c r="BB8" t="s">
+      <c r="BE8" t="s">
         <v>231</v>
       </c>
-      <c r="BC8" t="s">
+      <c r="BF8" t="s">
         <v>232</v>
       </c>
-      <c r="BD8" t="s">
+      <c r="BG8" t="s">
         <v>233</v>
       </c>
-      <c r="BE8" t="s">
+      <c r="BH8" t="s">
         <v>230</v>
       </c>
-      <c r="BF8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG8" t="s">
+      <c r="BI8" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ8" t="s">
         <v>425</v>
       </c>
-      <c r="BH8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BI8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ8" t="s">
-        <v>93</v>
-      </c>
       <c r="BK8" t="s">
         <v>93</v>
       </c>
@@ -3921,64 +3994,73 @@
         <v>93</v>
       </c>
       <c r="BO8" t="s">
+        <v>93</v>
+      </c>
+      <c r="BP8" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ8" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR8" t="s">
         <v>106</v>
       </c>
-      <c r="BP8" t="s">
+      <c r="BS8" t="s">
         <v>234</v>
       </c>
-      <c r="BQ8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BR8" t="b">
+      <c r="BT8" t="s">
+        <v>93</v>
+      </c>
+      <c r="BU8" t="b">
         <v>0</v>
       </c>
-      <c r="BS8" s="1" t="s">
+      <c r="BV8" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="BT8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BU8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BV8" t="s">
+      <c r="BW8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BX8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BY8" t="s">
         <v>348</v>
       </c>
-      <c r="BW8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BX8" s="1" t="s">
+      <c r="BZ8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CA8" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="BY8" s="1" t="s">
+      <c r="CB8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BZ8" t="s">
+      <c r="CC8" t="s">
         <v>342</v>
       </c>
-      <c r="CA8" s="1" t="s">
+      <c r="CD8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CB8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CC8" t="s">
-        <v>93</v>
-      </c>
-      <c r="CD8" s="1" t="s">
+      <c r="CE8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CF8" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG8" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="CE8" t="s">
+      <c r="CH8" t="s">
         <v>435</v>
       </c>
-      <c r="CF8" t="s">
-        <v>93</v>
-      </c>
-      <c r="CS8">
+      <c r="CI8" t="s">
+        <v>93</v>
+      </c>
+      <c r="CV8">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4009,93 +4091,93 @@
       <c r="J9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" t="s">
         <v>91</v>
       </c>
-      <c r="L9" t="s">
+      <c r="O9" t="s">
         <v>92</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="O9" t="s">
-        <v>93</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="Q9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R9" t="s">
+        <v>93</v>
+      </c>
+      <c r="S9" t="s">
         <v>238</v>
       </c>
-      <c r="Q9" t="s">
-        <v>93</v>
-      </c>
-      <c r="R9">
+      <c r="T9" t="s">
+        <v>93</v>
+      </c>
+      <c r="U9">
         <v>31423</v>
       </c>
-      <c r="S9" t="s">
+      <c r="V9" t="s">
         <v>239</v>
       </c>
-      <c r="T9" t="s">
+      <c r="W9" t="s">
         <v>240</v>
       </c>
-      <c r="U9" t="s">
+      <c r="X9" t="s">
         <v>329</v>
       </c>
-      <c r="V9" t="s">
+      <c r="Y9" t="s">
         <v>242</v>
       </c>
-      <c r="W9" t="s">
+      <c r="Z9" t="s">
         <v>243</v>
       </c>
-      <c r="X9" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>93</v>
-      </c>
       <c r="AA9" t="s">
         <v>93</v>
       </c>
       <c r="AB9" t="s">
         <v>93</v>
       </c>
-      <c r="AC9">
+      <c r="AC9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF9">
         <v>123421</v>
       </c>
-      <c r="AD9" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF9" t="s">
+      <c r="AG9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI9" t="s">
         <v>239</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AJ9" t="s">
         <v>240</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AK9" t="s">
         <v>241</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AL9" t="s">
         <v>242</v>
       </c>
-      <c r="AJ9">
+      <c r="AM9">
         <v>12341</v>
       </c>
-      <c r="AK9" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>93</v>
-      </c>
       <c r="AN9" t="s">
         <v>93</v>
       </c>
@@ -4109,56 +4191,56 @@
         <v>93</v>
       </c>
       <c r="AR9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU9" t="s">
         <v>398</v>
       </c>
-      <c r="AS9" t="s">
+      <c r="AV9" t="s">
         <v>101</v>
       </c>
-      <c r="AT9" t="s">
+      <c r="AW9" t="s">
         <v>407</v>
       </c>
-      <c r="AU9" t="s">
+      <c r="AX9" t="s">
         <v>101</v>
       </c>
-      <c r="AV9" t="s">
+      <c r="AY9" t="s">
         <v>412</v>
       </c>
-      <c r="AW9" t="s">
+      <c r="AZ9" t="s">
         <v>421</v>
       </c>
-      <c r="AX9" t="s">
+      <c r="BA9" t="s">
         <v>244</v>
       </c>
-      <c r="AY9" t="s">
+      <c r="BB9" t="s">
         <v>245</v>
       </c>
-      <c r="AZ9" s="3">
+      <c r="BC9" s="3">
         <v>43948</v>
       </c>
-      <c r="BA9" t="s">
+      <c r="BD9" t="s">
         <v>129</v>
       </c>
-      <c r="BB9" t="s">
+      <c r="BE9" t="s">
         <v>247</v>
       </c>
-      <c r="BC9" t="s">
+      <c r="BF9" t="s">
         <v>248</v>
       </c>
-      <c r="BD9" t="s">
+      <c r="BG9" t="s">
         <v>249</v>
       </c>
-      <c r="BE9" s="3">
+      <c r="BH9" s="3">
         <v>43948</v>
       </c>
-      <c r="BF9" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG9" t="s">
-        <v>93</v>
-      </c>
-      <c r="BH9" t="s">
-        <v>93</v>
-      </c>
       <c r="BI9" t="s">
         <v>93</v>
       </c>
@@ -4178,71 +4260,71 @@
         <v>93</v>
       </c>
       <c r="BO9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BP9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR9" t="s">
         <v>111</v>
       </c>
-      <c r="BP9" t="s">
-        <v>93</v>
-      </c>
-      <c r="BQ9" t="s">
+      <c r="BS9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BT9" t="s">
         <v>250</v>
       </c>
-      <c r="BR9" t="b">
+      <c r="BU9" t="b">
         <v>1</v>
       </c>
-      <c r="BS9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BT9" t="s">
-        <v>89</v>
-      </c>
-      <c r="BU9" t="s">
+      <c r="BV9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BW9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BX9" t="s">
         <v>90</v>
       </c>
-      <c r="BV9" t="s">
-        <v>93</v>
-      </c>
-      <c r="BW9" t="s">
-        <v>89</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>93</v>
-      </c>
-      <c r="BY9" s="1" t="s">
-        <v>89</v>
+      <c r="BY9" t="s">
+        <v>93</v>
       </c>
       <c r="BZ9" t="s">
-        <v>93</v>
-      </c>
-      <c r="CA9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CB9" t="s">
-        <v>89</v>
-      </c>
-      <c r="CC9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CA9" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CC9" t="s">
+        <v>93</v>
+      </c>
+      <c r="CD9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CE9" t="s">
+        <v>89</v>
+      </c>
+      <c r="CF9" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="CD9" s="1" t="s">
+      <c r="CG9" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="CE9" t="s">
+      <c r="CH9" t="s">
         <v>436</v>
       </c>
-      <c r="CF9" t="s">
+      <c r="CI9" t="s">
         <v>335</v>
       </c>
-      <c r="CI9" t="s">
+      <c r="CL9" t="s">
         <v>444</v>
       </c>
-      <c r="CJ9" t="s">
-        <v>93</v>
-      </c>
-      <c r="CK9" t="s">
-        <v>93</v>
-      </c>
-      <c r="CL9" t="s">
-        <v>93</v>
-      </c>
       <c r="CM9" t="s">
         <v>93</v>
       </c>
@@ -4258,8 +4340,17 @@
       <c r="CQ9" t="s">
         <v>93</v>
       </c>
+      <c r="CR9" t="s">
+        <v>93</v>
+      </c>
+      <c r="CS9" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT9" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4290,54 +4381,54 @@
       <c r="J10" t="s">
         <v>89</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
         <v>393</v>
       </c>
-      <c r="L10" t="s">
+      <c r="O10" t="s">
         <v>92</v>
       </c>
-      <c r="M10" t="s">
-        <v>93</v>
-      </c>
-      <c r="N10" t="s">
-        <v>89</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>89</v>
+      </c>
+      <c r="R10" t="s">
         <v>379</v>
       </c>
-      <c r="P10" t="s">
+      <c r="S10" t="s">
         <v>255</v>
       </c>
-      <c r="Q10" t="s">
-        <v>93</v>
-      </c>
-      <c r="R10" t="s">
-        <v>93</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
+        <v>93</v>
+      </c>
+      <c r="U10" t="s">
+        <v>93</v>
+      </c>
+      <c r="V10" t="s">
         <v>256</v>
       </c>
-      <c r="T10" t="s">
+      <c r="W10" t="s">
         <v>257</v>
       </c>
-      <c r="U10" t="s">
+      <c r="X10" t="s">
         <v>258</v>
       </c>
-      <c r="V10" t="s">
-        <v>93</v>
-      </c>
-      <c r="W10" t="s">
+      <c r="Y10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z10" t="s">
         <v>259</v>
       </c>
-      <c r="X10" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>93</v>
-      </c>
       <c r="AA10" t="s">
         <v>93</v>
       </c>
@@ -4354,29 +4445,29 @@
         <v>93</v>
       </c>
       <c r="AF10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI10" t="s">
         <v>260</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AJ10" t="s">
         <v>261</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AK10" t="s">
         <v>330</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AL10" t="s">
         <v>262</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AM10" t="s">
         <v>263</v>
       </c>
-      <c r="AK10" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>93</v>
-      </c>
       <c r="AN10" t="s">
         <v>93</v>
       </c>
@@ -4390,56 +4481,56 @@
         <v>93</v>
       </c>
       <c r="AR10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU10" t="s">
         <v>399</v>
       </c>
-      <c r="AS10" t="s">
+      <c r="AV10" t="s">
         <v>101</v>
       </c>
-      <c r="AT10" t="s">
+      <c r="AW10" t="s">
         <v>102</v>
       </c>
-      <c r="AU10" t="s">
+      <c r="AX10" t="s">
         <v>101</v>
       </c>
-      <c r="AV10" t="s">
+      <c r="AY10" t="s">
         <v>103</v>
       </c>
-      <c r="AW10" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX10" t="s">
+      <c r="AZ10" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA10" t="s">
         <v>264</v>
       </c>
-      <c r="AY10" t="s">
+      <c r="BB10" t="s">
         <v>265</v>
       </c>
-      <c r="AZ10" s="2">
+      <c r="BC10" s="2">
         <v>43948</v>
       </c>
-      <c r="BA10" t="s">
+      <c r="BD10" t="s">
         <v>129</v>
       </c>
-      <c r="BB10" t="s">
+      <c r="BE10" t="s">
         <v>266</v>
       </c>
-      <c r="BC10" t="s">
+      <c r="BF10" t="s">
         <v>267</v>
       </c>
-      <c r="BD10" t="s">
+      <c r="BG10" t="s">
         <v>268</v>
       </c>
-      <c r="BE10" s="2">
+      <c r="BH10" s="2">
         <v>43948</v>
       </c>
-      <c r="BF10" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG10" t="s">
-        <v>93</v>
-      </c>
-      <c r="BH10" t="s">
-        <v>93</v>
-      </c>
       <c r="BI10" t="s">
         <v>93</v>
       </c>
@@ -4456,94 +4547,103 @@
         <v>93</v>
       </c>
       <c r="BN10" t="s">
+        <v>93</v>
+      </c>
+      <c r="BO10" t="s">
+        <v>93</v>
+      </c>
+      <c r="BP10" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ10" t="s">
         <v>353</v>
       </c>
-      <c r="BO10" s="3">
+      <c r="BR10" s="3">
         <v>43947</v>
       </c>
-      <c r="BP10" t="s">
+      <c r="BS10" t="s">
         <v>269</v>
       </c>
-      <c r="BQ10" t="s">
+      <c r="BT10" t="s">
         <v>270</v>
       </c>
-      <c r="BR10" s="1" t="s">
+      <c r="BU10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BS10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BU10" t="s">
-        <v>89</v>
-      </c>
-      <c r="BV10" t="s">
+      <c r="BV10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BX10" t="s">
+        <v>89</v>
+      </c>
+      <c r="BY10" t="s">
         <v>349</v>
       </c>
-      <c r="BW10" t="s">
-        <v>89</v>
-      </c>
-      <c r="BX10" t="s">
-        <v>93</v>
-      </c>
-      <c r="BY10" t="s">
-        <v>89</v>
-      </c>
       <c r="BZ10" t="s">
+        <v>89</v>
+      </c>
+      <c r="CA10" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB10" t="s">
+        <v>89</v>
+      </c>
+      <c r="CC10" t="s">
         <v>343</v>
       </c>
-      <c r="CA10" t="s">
-        <v>89</v>
-      </c>
-      <c r="CB10" t="s">
-        <v>89</v>
-      </c>
       <c r="CD10" t="s">
+        <v>89</v>
+      </c>
+      <c r="CE10" t="s">
+        <v>89</v>
+      </c>
+      <c r="CG10" t="s">
         <v>427</v>
       </c>
-      <c r="CE10" t="s">
+      <c r="CH10" t="s">
         <v>437</v>
       </c>
-      <c r="CF10" t="s">
-        <v>93</v>
-      </c>
-      <c r="CG10" t="s">
+      <c r="CI10" t="s">
+        <v>93</v>
+      </c>
+      <c r="CJ10" t="s">
         <v>117</v>
       </c>
-      <c r="CH10" t="s">
+      <c r="CK10" t="s">
         <v>288</v>
       </c>
-      <c r="CI10" t="s">
+      <c r="CL10" t="s">
         <v>312</v>
       </c>
-      <c r="CJ10" t="s">
+      <c r="CM10" t="s">
         <v>324</v>
       </c>
-      <c r="CK10" s="3">
+      <c r="CN10" s="3">
         <v>43952</v>
       </c>
-      <c r="CL10" s="2">
+      <c r="CO10" s="2">
         <v>43958</v>
       </c>
-      <c r="CM10" t="s">
+      <c r="CP10" t="s">
         <v>325</v>
       </c>
-      <c r="CN10" t="s">
+      <c r="CQ10" t="s">
         <v>324</v>
       </c>
-      <c r="CO10" s="3">
+      <c r="CR10" s="3">
         <v>43958</v>
       </c>
-      <c r="CP10" s="2">
+      <c r="CS10" s="2">
         <v>43958</v>
       </c>
-      <c r="CQ10" t="s">
+      <c r="CT10" t="s">
         <v>321</v>
       </c>
-      <c r="CS10">
+      <c r="CV10">
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -4556,45 +4656,36 @@
       <c r="D11" t="s">
         <v>274</v>
       </c>
-      <c r="M11" t="s">
-        <v>93</v>
-      </c>
-      <c r="O11" t="s">
-        <v>93</v>
-      </c>
       <c r="P11" t="s">
+        <v>93</v>
+      </c>
+      <c r="R11" t="s">
+        <v>93</v>
+      </c>
+      <c r="S11" t="s">
         <v>275</v>
       </c>
-      <c r="Q11" t="s">
-        <v>93</v>
-      </c>
-      <c r="R11" t="s">
-        <v>93</v>
-      </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
+        <v>93</v>
+      </c>
+      <c r="U11" t="s">
+        <v>93</v>
+      </c>
+      <c r="V11" t="s">
         <v>276</v>
       </c>
-      <c r="T11" t="s">
+      <c r="W11" t="s">
         <v>277</v>
       </c>
-      <c r="U11" t="s">
+      <c r="X11" t="s">
         <v>278</v>
       </c>
-      <c r="V11" t="s">
-        <v>93</v>
-      </c>
-      <c r="W11">
+      <c r="Y11" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z11">
         <v>1231</v>
       </c>
-      <c r="X11" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>93</v>
-      </c>
       <c r="AA11" t="s">
         <v>93</v>
       </c>
@@ -4611,29 +4702,29 @@
         <v>93</v>
       </c>
       <c r="AF11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI11" t="s">
         <v>276</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AJ11" t="s">
         <v>277</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AK11" t="s">
         <v>278</v>
       </c>
-      <c r="AI11" t="s">
-        <v>93</v>
-      </c>
-      <c r="AJ11" t="s">
+      <c r="AL11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM11" t="s">
         <v>279</v>
       </c>
-      <c r="AK11" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>93</v>
-      </c>
       <c r="AN11" t="s">
         <v>93</v>
       </c>
@@ -4647,143 +4738,143 @@
         <v>93</v>
       </c>
       <c r="AR11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU11" t="s">
         <v>400</v>
       </c>
-      <c r="AS11" t="s">
+      <c r="AV11" t="s">
         <v>101</v>
       </c>
-      <c r="AT11" t="s">
+      <c r="AW11" t="s">
         <v>103</v>
       </c>
-      <c r="AU11" t="s">
+      <c r="AX11" t="s">
         <v>101</v>
       </c>
-      <c r="AV11" t="s">
+      <c r="AY11" t="s">
         <v>413</v>
       </c>
-      <c r="AW11" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX11" t="s">
+      <c r="AZ11" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA11" t="s">
         <v>280</v>
       </c>
-      <c r="AY11" t="s">
+      <c r="BB11" t="s">
         <v>281</v>
       </c>
-      <c r="AZ11" t="s">
+      <c r="BC11" t="s">
         <v>246</v>
       </c>
-      <c r="BA11" t="s">
+      <c r="BD11" t="s">
         <v>129</v>
       </c>
-      <c r="BB11" t="s">
+      <c r="BE11" t="s">
         <v>282</v>
       </c>
-      <c r="BC11" t="s">
+      <c r="BF11" t="s">
         <v>283</v>
       </c>
-      <c r="BD11" t="s">
+      <c r="BG11" t="s">
         <v>284</v>
       </c>
-      <c r="BE11" t="s">
+      <c r="BH11" t="s">
         <v>246</v>
       </c>
-      <c r="BF11" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG11" t="s">
+      <c r="BI11" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ11" t="s">
         <v>133</v>
       </c>
-      <c r="BH11" t="s">
+      <c r="BK11" t="s">
         <v>285</v>
       </c>
-      <c r="BJ11" t="s">
+      <c r="BM11" t="s">
         <v>286</v>
       </c>
-      <c r="BK11" t="s">
+      <c r="BN11" t="s">
         <v>287</v>
       </c>
-      <c r="BL11" t="s">
+      <c r="BO11" t="s">
         <v>137</v>
       </c>
-      <c r="BM11" t="s">
+      <c r="BP11" t="s">
         <v>288</v>
       </c>
-      <c r="BN11" t="s">
-        <v>93</v>
-      </c>
-      <c r="BO11" t="s">
+      <c r="BQ11" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR11" t="s">
         <v>106</v>
       </c>
-      <c r="BP11" t="s">
-        <v>93</v>
-      </c>
-      <c r="BQ11" t="s">
+      <c r="BS11" t="s">
+        <v>93</v>
+      </c>
+      <c r="BT11" t="s">
         <v>289</v>
       </c>
-      <c r="BR11" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BS11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BT11" t="s">
-        <v>89</v>
-      </c>
-      <c r="BU11" t="s">
+      <c r="BU11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BW11" t="s">
+        <v>89</v>
+      </c>
+      <c r="BX11" t="s">
         <v>90</v>
       </c>
-      <c r="BV11" t="s">
-        <v>93</v>
-      </c>
-      <c r="BW11" t="s">
-        <v>89</v>
-      </c>
-      <c r="BX11" t="s">
+      <c r="BY11" t="s">
+        <v>93</v>
+      </c>
+      <c r="BZ11" t="s">
+        <v>89</v>
+      </c>
+      <c r="CA11" t="s">
         <v>346</v>
       </c>
-      <c r="BY11" t="s">
+      <c r="CB11" t="s">
         <v>90</v>
       </c>
-      <c r="BZ11" t="s">
-        <v>93</v>
-      </c>
-      <c r="CA11" t="s">
-        <v>89</v>
-      </c>
-      <c r="CB11" t="s">
-        <v>89</v>
-      </c>
       <c r="CC11" t="s">
         <v>93</v>
       </c>
       <c r="CD11" t="s">
+        <v>89</v>
+      </c>
+      <c r="CE11" t="s">
+        <v>89</v>
+      </c>
+      <c r="CF11" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG11" t="s">
         <v>428</v>
       </c>
-      <c r="CE11" t="s">
+      <c r="CH11" t="s">
         <v>438</v>
       </c>
-      <c r="CF11" t="s">
+      <c r="CI11" t="s">
         <v>336</v>
       </c>
-      <c r="CG11" t="s">
+      <c r="CJ11" t="s">
         <v>117</v>
       </c>
-      <c r="CH11" t="s">
-        <v>93</v>
-      </c>
-      <c r="CI11" t="s">
+      <c r="CK11" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL11" t="s">
         <v>443</v>
       </c>
-      <c r="CJ11" t="s">
-        <v>93</v>
-      </c>
-      <c r="CK11" t="s">
-        <v>93</v>
-      </c>
-      <c r="CL11" t="s">
-        <v>93</v>
-      </c>
       <c r="CM11" t="s">
         <v>93</v>
       </c>
@@ -4799,8 +4890,17 @@
       <c r="CQ11" t="s">
         <v>93</v>
       </c>
+      <c r="CR11" t="s">
+        <v>93</v>
+      </c>
+      <c r="CS11" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT11" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>
@@ -4831,85 +4931,94 @@
       <c r="J12" t="s">
         <v>90</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
         <v>395</v>
       </c>
-      <c r="L12" t="s">
+      <c r="O12" t="s">
         <v>92</v>
       </c>
-      <c r="M12" t="s">
-        <v>93</v>
-      </c>
-      <c r="N12" t="s">
-        <v>89</v>
-      </c>
-      <c r="O12" t="s">
-        <v>93</v>
-      </c>
       <c r="P12" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>89</v>
+      </c>
+      <c r="R12" t="s">
+        <v>93</v>
+      </c>
+      <c r="S12" t="s">
         <v>386</v>
       </c>
-      <c r="Q12" t="s">
-        <v>93</v>
-      </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
+        <v>93</v>
+      </c>
+      <c r="V12" t="s">
         <v>297</v>
       </c>
-      <c r="T12" t="s">
+      <c r="W12" t="s">
         <v>298</v>
       </c>
-      <c r="U12" t="s">
+      <c r="X12" t="s">
         <v>299</v>
       </c>
-      <c r="W12" t="s">
+      <c r="Z12" t="s">
         <v>300</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AI12" t="s">
         <v>297</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AJ12" t="s">
         <v>298</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AK12" t="s">
         <v>331</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AM12" t="s">
         <v>300</v>
       </c>
-      <c r="AR12" t="s">
+      <c r="AU12" t="s">
         <v>371</v>
       </c>
-      <c r="AS12" t="s">
+      <c r="AV12" t="s">
         <v>101</v>
       </c>
-      <c r="AT12" t="s">
+      <c r="AW12" t="s">
         <v>409</v>
       </c>
-      <c r="AU12" t="s">
+      <c r="AX12" t="s">
         <v>101</v>
       </c>
-      <c r="AV12" t="s">
+      <c r="AY12" t="s">
         <v>414</v>
       </c>
-      <c r="BO12" t="s">
+      <c r="BR12" t="s">
         <v>111</v>
       </c>
-      <c r="CH12" t="s">
+      <c r="CK12" t="s">
         <v>319</v>
       </c>
-      <c r="CI12" t="s">
+      <c r="CL12" t="s">
         <v>442</v>
       </c>
-      <c r="CJ12" t="s">
+      <c r="CM12" t="s">
         <v>322</v>
       </c>
-      <c r="CK12" t="s">
+      <c r="CN12" t="s">
         <v>214</v>
       </c>
-      <c r="CL12" t="s">
+      <c r="CO12" t="s">
         <v>311</v>
       </c>
-      <c r="CM12" t="s">
+      <c r="CP12" t="s">
         <v>321</v>
       </c>
     </row>
@@ -4917,7 +5026,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <ignoredErrors>
-    <ignoredError sqref="AU6 AS6" numberStoredAsText="1"/>
+    <ignoredError sqref="AX6 AV6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>